<commit_message>
Updated IG with the latest files from output
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-SiteQualifier.xlsx
+++ b/docs/StructureDefinition-SiteQualifier.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-04-29T20:38:23+02:00</t>
+    <t>2025-05-05T10:23:37+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -129,7 +129,7 @@
     <t>Context</t>
   </si>
   <si>
-    <t>element:http://example.org/StructureDefinition/my-MyDosage#MedicationAdministration</t>
+    <t>element:http://example.org/StructureDefinition/my-MyDosageAdministration#MedicationAdministration</t>
   </si>
   <si>
     <t>ID</t>

</xml_diff>